<commit_message>
Annina's questions to data cleaning and OLS first try
</commit_message>
<xml_diff>
--- a/dictionary_metadata_columnsnames.xlsx
+++ b/dictionary_metadata_columnsnames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anninamack/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anninamack/Desktop/St.Gallen/HSG/HS2022/DSF/Project-Disney-World-DSF/Project-Disney-World-DSF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4D88C1-2DAF-FD45-B5FB-B6FD5F66A348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00675B5-95F6-CF40-92C5-30B856505432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="5" r:id="rId1"/>
@@ -22,6 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">metadata!$A$1:$D$191</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">metadata!$B$1:$B$191</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -2879,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3027,6 +3028,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3135,6 +3137,7 @@
     <mergeCell ref="B6:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3142,9 +3145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5830,7 +5833,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B191" xr:uid="{7BB245EA-FA39-0D40-9762-87D8F9D85400}">
+      <formula1>","</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5928,6 +5938,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6255,6 +6266,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6918,5 +6930,6 @@
     <sortCondition ref="A2:A80"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>